<commit_message>
Tiny correction in some numbers in the data insertion script.
</commit_message>
<xml_diff>
--- a/design/eco_data_irrigation_range.xlsx
+++ b/design/eco_data_irrigation_range.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Documents\Git\UBICUA\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C4789B-05E0-4646-897F-5EB7F05319F4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC82229D-21BA-408A-A7F5-EFC64A722CF8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{2F03C95B-DEDF-4142-817B-2CDAA4355F09}"/>
   </bookViews>
@@ -31,15 +31,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>ID</t>
   </si>
   <si>
     <t>FAMILY_ID</t>
-  </si>
-  <si>
-    <t>0.8</t>
   </si>
   <si>
     <t>TEMP_EXT_HIGHER_LIMIT</t>
@@ -412,7 +409,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,19 +429,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -454,11 +451,11 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
+      <c r="C2">
+        <v>28</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <v>80</v>
@@ -467,11 +464,11 @@
         <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H2" t="str">
         <f>_xlfn.CONCAT("INSERT INTO IRRIGATION_RANGE (ID, FAMILY_ID, TEMP_EXT_HIGHER_LIMIT, TEMP_EXT_LOWER_LIMIT, HUM_EXT_HIGHER_LIMIT, HUM_EXT_LOWER_LIMIT, LUMINOSITY_LIMIT) VALUES (", A2,", ", B2,", ",C2,", ",D2,", ",E2,", ",F2,", ",G2,");")</f>
-        <v>INSERT INTO IRRIGATION_RANGE (ID, FAMILY_ID, TEMP_EXT_HIGHER_LIMIT, TEMP_EXT_LOWER_LIMIT, HUM_EXT_HIGHER_LIMIT, HUM_EXT_LOWER_LIMIT, LUMINOSITY_LIMIT) VALUES (1, 1, 0.8, 1, 80, 40, 0.5);</v>
+        <v>INSERT INTO IRRIGATION_RANGE (ID, FAMILY_ID, TEMP_EXT_HIGHER_LIMIT, TEMP_EXT_LOWER_LIMIT, HUM_EXT_HIGHER_LIMIT, HUM_EXT_LOWER_LIMIT, LUMINOSITY_LIMIT) VALUES (1, 1, 28, 10, 80, 40, 0.5);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>